<commit_message>
rm useless short c6a6e8b9e0c5658dfc67adebe0b621246c138f50
</commit_message>
<xml_diff>
--- a/nr-add-st/ig/StructureDefinition-cdl-document-reference.xlsx
+++ b/nr-add-st/ig/StructureDefinition-cdl-document-reference.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-26T11:55:14+00:00</t>
+    <t>2024-06-26T11:56:25+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -630,7 +630,7 @@
 </t>
   </si>
   <si>
-    <t>Kind of document</t>
+    <t>Kind of document (LOINC if possible)</t>
   </si>
   <si>
     <t>Specifies the particular kind of document referenced  (e.g. History and Physical, Discharge Summary, Progress Note). This usually equates to the purpose of making the document referenced.</t>

</xml_diff>

<commit_message>
add mapping mos d0e6af4e1a755a602cff1d6b9200d32df615fb97
</commit_message>
<xml_diff>
--- a/nr-add-st/ig/StructureDefinition-cdl-document-reference.xlsx
+++ b/nr-add-st/ig/StructureDefinition-cdl-document-reference.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-07-17T12:07:37+00:00</t>
+    <t>2024-07-22T08:11:32+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -810,7 +810,7 @@
     <t>Not necessarily who did the actual data entry (i.e. typist) or who was the source (informant).</t>
   </si>
   <si>
-    <t>Note.auteurNote</t>
+    <t>AuteurNote.idAuteurNote</t>
   </si>
   <si>
     <t>Event.performer.actor</t>

</xml_diff>